<commit_message>
return all column in get function
added setup function in test case

modified spreadsheet fixture
</commit_message>
<xml_diff>
--- a/test/Fixture/DataAccessor/SampleEmptySheet.xlsx
+++ b/test/Fixture/DataAccessor/SampleEmptySheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24990"/>
   </bookViews>
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>id1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -370,58 +358,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -431,7 +375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -439,7 +383,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>